<commit_message>
exporting analysis result excel files
</commit_message>
<xml_diff>
--- a/sidekick/resources/rdata/rep_HCC_T_vs_Normal_3x.xlsx
+++ b/sidekick/resources/rdata/rep_HCC_T_vs_Normal_3x.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jigsaw-0/Workspace/SNU-BIOINFO/Projects/NASH_HCC_Liver-KRIBB_2022/sidekick/resources/rdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C9924D9F-8314-9E44-961B-9C621B1A2157}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E72A9AA-B24F-B545-B1FE-F5A0F6E4159A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="760" windowWidth="23540" windowHeight="15280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -10821,7 +10821,7 @@
   <dimension ref="A1:D3466"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>